<commit_message>
fixed (?) reification model changes
</commit_message>
<xml_diff>
--- a/common/src/test/resources/test12.xlsx
+++ b/common/src/test/resources/test12.xlsx
@@ -5,13 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Purchases" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Humans" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -131,13 +136,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -176,19 +177,17 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="35.05"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.71255060728745"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -201,11 +200,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -218,7 +217,7 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="2" t="n">
         <v>41952</v>
       </c>
     </row>
@@ -246,36 +245,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
settled on subPropertyOf for reifying edges
</commit_message>
<xml_diff>
--- a/common/src/test/resources/test12.xlsx
+++ b/common/src/test/resources/test12.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Relation</t>
   </si>
@@ -50,6 +50,21 @@
     <t>3000 USD</t>
   </si>
   <si>
+    <t># F2 is a comment</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>Cadillac</t>
+  </si>
+  <si>
+    <t>#D3 is a comment</t>
+  </si>
+  <si>
+    <t>#A4 is a comment</t>
+  </si>
+  <si>
     <t>Node</t>
   </si>
   <si>
@@ -60,15 +75,19 @@
   </si>
   <si>
     <t>Gargarin</t>
+  </si>
+  <si>
+    <t>Shepard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -136,7 +155,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,6 +165,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,17 +197,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.05"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.0607287449393"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -219,6 +242,26 @@
       </c>
       <c r="E2" s="2" t="n">
         <v>41952</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -237,45 +280,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>